<commit_message>
20220119 update kubernetes doc
</commit_message>
<xml_diff>
--- a/Kubernetes.xlsx
+++ b/Kubernetes.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
@@ -11,12 +11,12 @@
     <sheet name="command" sheetId="1" r:id="rId2"/>
     <sheet name="command_linux" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" calcMode="manual"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="223">
   <si>
     <t>node&amp;pod確認</t>
     <rPh sb="8" eb="10">
@@ -1848,12 +1848,475 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>StatefulSet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Object</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pod, DeploymentはSpec, statusなどの値をもっているが、このような値を持っているPodとDeploymentを</t>
+    <rPh sb="31" eb="32">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>アタイ</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>個別属性を含めた単位を</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Object</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>と言う。</t>
+    </r>
+    <rPh sb="0" eb="2">
+      <t>コベツ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ゾクセイ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>フク</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>タンイ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>イ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>基本Object</t>
+    <rPh sb="0" eb="2">
+      <t>キホン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・Pod：Kubernetesの中で実行される最小単位、つまりWeb Serviceの稼働に必要な最小単位。</t>
+    <rPh sb="16" eb="17">
+      <t>ナカ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ジッコウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>サイショウ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>タンイ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>カドウ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="49" eb="51">
+      <t>サイショウ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>タンイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>１つのPodは１つ以上のContainerを持つ。</t>
+    <rPh sb="9" eb="11">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・Namespace：Resourceを区別して管理するグループ</t>
+    <rPh sb="20" eb="22">
+      <t>クベツ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>カンリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>指定なしの場合は「default」、kubernetes systemで使用されるkube-systemなど</t>
+    <rPh sb="0" eb="2">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="36" eb="38">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・Volume：Podが生成されるときにPodに必要なDirectoryを提供</t>
+    <rPh sb="12" eb="14">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>テイキョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>・Service：Pod接続を安定的に維持できるようにServiceを通して内・外部に通信する。</t>
+    <rPh sb="12" eb="14">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="15" eb="18">
+      <t>アンテイテキ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>イジ</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>トオ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ナイ</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>ガイ</t>
+    </rPh>
+    <rPh sb="41" eb="42">
+      <t>ブ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>ツウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Kubernetesの外部からKubernetes内部に接続するとき、内部がどういった構造になっているか、Podは動いているか気にしなくても</t>
+    <rPh sb="11" eb="13">
+      <t>ガイブ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ナイブ</t>
+    </rPh>
+    <rPh sb="43" eb="45">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="57" eb="58">
+      <t>ウゴ</t>
+    </rPh>
+    <rPh sb="63" eb="64">
+      <t>キ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>論理的にKubernetesの内部につなぐのService。</t>
+    <rPh sb="0" eb="3">
+      <t>ロンリテキ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>ナイブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>既存インフラで言うと、LoaderBalancer、Gatewayのような役割。</t>
+    <rPh sb="0" eb="2">
+      <t>キゾン</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>ヤクワリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Deployment</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>機能を組み立てたり追加したりしてもっと効率よく稼働できるようにする。</t>
+    <rPh sb="0" eb="2">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ク</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ツイカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ownerReferences</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DeploymentのObject layer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Deployment生成監視</t>
+    <rPh sb="10" eb="12">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カンシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReplicaSet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReplicaSet　生成</t>
+    <rPh sb="11" eb="13">
+      <t>セイセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReplicaSet生成監視</t>
+    <rPh sb="10" eb="12">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カンシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ReplicaSetで宣言した</t>
+    <rPh sb="11" eb="13">
+      <t>センゲン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pod(s) 生成</t>
+    <rPh sb="7" eb="9">
+      <t>セイセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>API ServerとControleer Managerの通信</t>
+    <rPh sb="30" eb="32">
+      <t>ツウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Podの数を管理するObject</t>
+    <rPh sb="4" eb="5">
+      <t>カズ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>カンリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※drain解除：kubectl uncordon &lt;node名&gt;</t>
+    <rPh sb="6" eb="8">
+      <t>カイジョ</t>
+    </rPh>
+    <rPh sb="31" eb="32">
+      <t>メイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Service</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>外部からKubernetes Clusterへ接続する方法</t>
+    <rPh sb="0" eb="2">
+      <t>ガイブ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>ホウホウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NodePort</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>全てのWorkerNodeが特定のPortを開けてそのPortから入ってくるリクエストは全てNodePort serviceに連携し、</t>
+    <rPh sb="0" eb="1">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>トクテイ</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="44" eb="45">
+      <t>スベ</t>
+    </rPh>
+    <rPh sb="63" eb="65">
+      <t>レンケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NodePort Serviceは該当タスクを処理できるPodにRequestを連携する（再振分け）</t>
+    <rPh sb="17" eb="19">
+      <t>ガイトウ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="40" eb="42">
+      <t>レンケイ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>サイ</t>
+    </rPh>
+    <rPh sb="46" eb="48">
+      <t>フリワ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NodePort Service 構成</t>
+    <rPh sb="17" eb="19">
+      <t>コウセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>targetPort:80</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>NodePort:30000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>hostIP:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30000</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>で接続</t>
+    </r>
+    <rPh sb="13" eb="15">
+      <t>セツゾク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>←外部からアクセスするPort</t>
+    <rPh sb="1" eb="3">
+      <t>ガイブ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>←NodePortがPodに連携するPort</t>
+    <rPh sb="14" eb="16">
+      <t>レンケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ingress</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※Portの重複使用は不可。そのため、１つのNodePortに１つのDeploymentだけが適用される</t>
+    <rPh sb="6" eb="8">
+      <t>チョウフク</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>フカ</t>
+    </rPh>
+    <rPh sb="47" eb="49">
+      <t>テキヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1912,6 +2375,22 @@
     </font>
     <font>
       <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="16"/>
       <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -1989,15 +2468,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -3372,8 +3853,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3288254" y="5397649"/>
-          <a:ext cx="895574" cy="495749"/>
+          <a:off x="3288254" y="7549179"/>
+          <a:ext cx="895574" cy="710901"/>
           <a:chOff x="3436620" y="4907280"/>
           <a:chExt cx="914400" cy="487680"/>
         </a:xfrm>
@@ -3506,8 +3987,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3286349" y="6689015"/>
-          <a:ext cx="883024" cy="495749"/>
+          <a:off x="3286349" y="9342568"/>
+          <a:ext cx="883024" cy="710901"/>
           <a:chOff x="3436620" y="4907280"/>
           <a:chExt cx="914400" cy="487680"/>
         </a:xfrm>
@@ -4561,8 +5042,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5714440" y="5621319"/>
-          <a:ext cx="4005542" cy="1067696"/>
+          <a:off x="5714440" y="7844566"/>
+          <a:ext cx="4005542" cy="1498002"/>
           <a:chOff x="5827395" y="4983480"/>
           <a:chExt cx="4086225" cy="1051560"/>
         </a:xfrm>
@@ -5323,8 +5804,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5722060" y="6945854"/>
-          <a:ext cx="4005542" cy="1067697"/>
+          <a:off x="5722060" y="9742842"/>
+          <a:ext cx="4005542" cy="1498003"/>
           <a:chOff x="5827395" y="4983480"/>
           <a:chExt cx="4086225" cy="1051560"/>
         </a:xfrm>
@@ -6085,8 +6566,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="5722060" y="8221980"/>
-          <a:ext cx="4005542" cy="1070386"/>
+          <a:off x="5722060" y="11520992"/>
+          <a:ext cx="4005542" cy="1572409"/>
           <a:chOff x="5827395" y="4983480"/>
           <a:chExt cx="4086225" cy="1051560"/>
         </a:xfrm>
@@ -7284,8 +7765,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="8532607" y="4345193"/>
-          <a:ext cx="1156895" cy="1090556"/>
+          <a:off x="8532607" y="6066416"/>
+          <a:ext cx="1156895" cy="1520863"/>
           <a:chOff x="8366760" y="3779520"/>
           <a:chExt cx="1181100" cy="1074420"/>
         </a:xfrm>
@@ -8825,8 +9306,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1093693" y="16880541"/>
-          <a:ext cx="526452" cy="851647"/>
+          <a:off x="1093693" y="23765435"/>
+          <a:ext cx="526452" cy="1210235"/>
           <a:chOff x="1210235" y="16324729"/>
           <a:chExt cx="526452" cy="851647"/>
         </a:xfrm>
@@ -8994,8 +9475,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="860612" y="17803905"/>
-          <a:ext cx="1004046" cy="600635"/>
+          <a:off x="860612" y="25047387"/>
+          <a:ext cx="1004046" cy="887506"/>
           <a:chOff x="3436620" y="4907280"/>
           <a:chExt cx="914400" cy="460205"/>
         </a:xfrm>
@@ -9275,8 +9756,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2823877" y="17391529"/>
-          <a:ext cx="773930" cy="493059"/>
+          <a:off x="2823877" y="24491576"/>
+          <a:ext cx="773930" cy="708212"/>
           <a:chOff x="2967317" y="17391529"/>
           <a:chExt cx="773930" cy="493059"/>
         </a:xfrm>
@@ -9582,8 +10063,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3307976" y="15419294"/>
-          <a:ext cx="773930" cy="493059"/>
+          <a:off x="3307976" y="21658729"/>
+          <a:ext cx="773930" cy="708212"/>
           <a:chOff x="2967317" y="17391529"/>
           <a:chExt cx="773930" cy="493059"/>
         </a:xfrm>
@@ -11691,8 +12172,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7817224" y="18153529"/>
-          <a:ext cx="881406" cy="495164"/>
+          <a:off x="7817224" y="25540446"/>
+          <a:ext cx="881406" cy="710317"/>
           <a:chOff x="12102353" y="7055224"/>
           <a:chExt cx="881406" cy="495164"/>
         </a:xfrm>
@@ -11948,8 +12429,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10255621" y="17866659"/>
-          <a:ext cx="1694329" cy="1281954"/>
+          <a:off x="10255621" y="25181859"/>
+          <a:ext cx="1694329" cy="1783978"/>
           <a:chOff x="9314329" y="15015883"/>
           <a:chExt cx="1694329" cy="1281954"/>
         </a:xfrm>
@@ -13308,6 +13789,2826 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>35859</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>215152</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>233083</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="227" name="모서리가 둥근 직사각형 226"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="708212" y="36038117"/>
+          <a:ext cx="1712260" cy="502025"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Deployment</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>35858</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>35858</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>53789</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="199" name="모서리가 둥근 직사각형 198"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="708211" y="36827011"/>
+          <a:ext cx="1712260" cy="502025"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ReplicaSet</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>(</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>旧</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ReplicationController)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>53788</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>80684</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>80683</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>53788</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="200" name="모서리가 둥근 직사각형 199"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="860612" y="37355931"/>
+          <a:ext cx="1371600" cy="215151"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>replicas: 1</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>62753</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>116541</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="228" name="직사각형 227"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2554941" y="37911741"/>
+          <a:ext cx="869577" cy="448235"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>POD</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>224117</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>62753</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>188258</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="202" name="직사각형 201"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2554941" y="38709599"/>
+          <a:ext cx="869577" cy="448235"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>POD</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>67236</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>53787</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>134470</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="232" name="꺾인 연결선 231"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="200" idx="2"/>
+          <a:endCxn id="228" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1768288" y="37349205"/>
+          <a:ext cx="564777" cy="1008529"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>67236</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>53787</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>206187</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="205" name="꺾인 연결선 204"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="200" idx="2"/>
+          <a:endCxn id="202" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1369359" y="37748134"/>
+          <a:ext cx="1362635" cy="1008529"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>62753</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="211" name="꺾인 연결선 210"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="228" idx="3"/>
+          <a:endCxn id="199" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2420471" y="37078024"/>
+          <a:ext cx="1004047" cy="1057835"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -22768"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>62753</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>75453</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>206188</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="212" name="꺾인 연결선 211"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="202" idx="3"/>
+          <a:endCxn id="228" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="3424518" y="38135859"/>
+          <a:ext cx="12700" cy="797858"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 1800000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="sysDash"/>
+          <a:tailEnd type="none"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85165</xdr:colOff>
+      <xdr:row>150</xdr:row>
+      <xdr:rowOff>233083</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85166</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>35858</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="247" name="직선 화살표 연결선 246"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="227" idx="2"/>
+          <a:endCxn id="199" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="1564341" y="36540142"/>
+          <a:ext cx="1" cy="286869"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>17930</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>71717</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>119507</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>53788</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="220" name="그룹 219"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="4455459" y="35894682"/>
+          <a:ext cx="773930" cy="708212"/>
+          <a:chOff x="2967317" y="17391529"/>
+          <a:chExt cx="773930" cy="493059"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="221" name="육각형 220"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3012142" y="17391529"/>
+            <a:ext cx="645458" cy="493059"/>
+          </a:xfrm>
+          <a:prstGeom prst="hexagon">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="222" name="TextBox 221"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2967317" y="17517036"/>
+            <a:ext cx="773930" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>API</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1050" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Server</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1050">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>8964</xdr:colOff>
+      <xdr:row>148</xdr:row>
+      <xdr:rowOff>71717</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>107576</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>35858</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="255" name="육각형 254"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6598023" y="35894682"/>
+          <a:ext cx="905435" cy="690282"/>
+        </a:xfrm>
+        <a:prstGeom prst="hexagon">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800"/>
+            <a:t>Controller</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800" baseline="0"/>
+            <a:t> Manager</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>107576</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>71718</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>107576</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="257" name="직선 연결선 256"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4814047" y="36620824"/>
+          <a:ext cx="0" cy="2528047"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>62750</xdr:colOff>
+      <xdr:row>151</xdr:row>
+      <xdr:rowOff>71718</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>62750</xdr:colOff>
+      <xdr:row>161</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="258" name="직선 연결선 257"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7055221" y="36620824"/>
+          <a:ext cx="0" cy="2528047"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="22225">
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="sysDash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>44823</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>26894</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>215153</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="259" name="직사각형 258"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4751294" y="37409718"/>
+          <a:ext cx="116541" cy="322729"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>44823</xdr:colOff>
+      <xdr:row>158</xdr:row>
+      <xdr:rowOff>116542</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>26894</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>197224</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="260" name="직사각형 259"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4751294" y="38359977"/>
+          <a:ext cx="116541" cy="322729"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>116540</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>35859</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>125500</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>35861</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="261" name="직선 화살표 연결선 260"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4823011" y="37069059"/>
+          <a:ext cx="2160489" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>125505</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>35860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>116541</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>215154</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="262" name="직사각형 261"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6983505" y="37069060"/>
+          <a:ext cx="125507" cy="663388"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>125505</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>35862</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>52</xdr:col>
+      <xdr:colOff>116541</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>215156</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="263" name="직사각형 262"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6983505" y="38037250"/>
+          <a:ext cx="125507" cy="663388"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg2">
+            <a:lumMod val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>26894</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>53788</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>107576</xdr:colOff>
+      <xdr:row>155</xdr:row>
+      <xdr:rowOff>53789</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="264" name="직선 화살표 연결선 263"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="259" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4867835" y="37571082"/>
+          <a:ext cx="2097741" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>116540</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>125500</xdr:colOff>
+      <xdr:row>157</xdr:row>
+      <xdr:rowOff>44826</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="265" name="직선 화살표 연결선 264"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4823011" y="38046212"/>
+          <a:ext cx="2160489" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>26894</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>107576</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>44825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="266" name="직선 화살표 연결선 265"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4867835" y="38530306"/>
+          <a:ext cx="2097741" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>17931</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>44824</xdr:colOff>
+      <xdr:row>186</xdr:row>
+      <xdr:rowOff>197224</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="341" name="그룹 340"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="672352" y="42376166"/>
+          <a:ext cx="5423648" cy="2841811"/>
+          <a:chOff x="1084728" y="41972754"/>
+          <a:chExt cx="5423648" cy="2841811"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="268" name="직사각형 267"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1084728" y="43182987"/>
+            <a:ext cx="5423648" cy="412377"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>NodePort Service</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="269" name="직사각형 268"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1084728" y="43604329"/>
+            <a:ext cx="5423648" cy="1210236"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="270" name="직사각형 269"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1183341" y="44025672"/>
+            <a:ext cx="1721224" cy="708212"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Port(80:30000/TCP)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Worker Node #1</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="271" name="직사각형 270"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2976281" y="44025672"/>
+            <a:ext cx="1712259" cy="708212"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Port(80:30000/TCP)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Worker Node #1</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="272" name="직사각형 271"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4760259" y="44025672"/>
+            <a:ext cx="1676399" cy="708212"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Port(80:30000/TCP)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Worker Node #1</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="273" name="그룹 272"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="1264024" y="41972754"/>
+            <a:ext cx="526452" cy="959223"/>
+            <a:chOff x="1210235" y="16324729"/>
+            <a:chExt cx="526452" cy="851647"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="274" name="순서도: 지연 273"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="16200000">
+              <a:off x="1284081" y="16750441"/>
+              <a:ext cx="352089" cy="499782"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartDelay">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="275" name="타원 274"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1272315" y="16517918"/>
+              <a:ext cx="388172" cy="371139"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="276" name="TextBox 275"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1244525" y="16324729"/>
+              <a:ext cx="492162" cy="216049"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>User</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="277" name="꺾인 연결선 276"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="274" idx="1"/>
+            <a:endCxn id="78" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="862295" y="43365084"/>
+            <a:ext cx="1084727" cy="218515"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 65703"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="280" name="꺾인 연결선 279"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="274" idx="1"/>
+            <a:endCxn id="289" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1754283" y="42691610"/>
+            <a:ext cx="1084727" cy="1565462"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 65703"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="283" name="꺾인 연결선 282"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="274" idx="1"/>
+            <a:endCxn id="290" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="2650753" y="41795139"/>
+            <a:ext cx="1084727" cy="3358403"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 65703"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="76" name="TextBox 75"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1506071" y="42958871"/>
+            <a:ext cx="325730" cy="275717"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+              <a:t>①</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="288" name="꺾인 연결선 287"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="270" idx="0"/>
+            <a:endCxn id="269" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000" flipH="1" flipV="1">
+            <a:off x="2709581" y="42938702"/>
+            <a:ext cx="421343" cy="1752599"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 56383"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="78" name="타원 77"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1201271" y="44016705"/>
+            <a:ext cx="188258" cy="206188"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="289" name="타원 288"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2985248" y="44016705"/>
+            <a:ext cx="188258" cy="206188"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="290" name="타원 289"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4778189" y="44016705"/>
+            <a:ext cx="188258" cy="206188"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="309" name="꺾인 연결선 308"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="271" idx="0"/>
+            <a:endCxn id="269" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipV="1">
+            <a:off x="3603811" y="43797071"/>
+            <a:ext cx="421343" cy="35859"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 52128"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="313" name="꺾인 연결선 312"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="272" idx="0"/>
+            <a:endCxn id="269" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipV="1">
+            <a:off x="4486835" y="42914047"/>
+            <a:ext cx="421343" cy="1801907"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 54255"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="317" name="TextBox 316"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1748118" y="43747765"/>
+            <a:ext cx="325730" cy="275717"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>②</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="318" name="직사각형 317"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2357718" y="44375295"/>
+            <a:ext cx="555812" cy="349624"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>POD</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="319" name="직사각형 318"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4114801" y="44375295"/>
+            <a:ext cx="555812" cy="349624"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>POD</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="320" name="직사각형 319"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5880848" y="44375295"/>
+            <a:ext cx="555812" cy="349624"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>POD</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="321" name="꺾인 연결선 320"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="324" idx="2"/>
+            <a:endCxn id="320" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="5219699" y="43436240"/>
+            <a:ext cx="869578" cy="1008531"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 42784"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="dashDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="324" name="직사각형 323"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4670611" y="43254705"/>
+            <a:ext cx="959224" cy="251012"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>③再振分け</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="328" name="꺾인 연결선 327"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="324" idx="2"/>
+            <a:endCxn id="319" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="4336676" y="43561748"/>
+            <a:ext cx="869578" cy="757516"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 42784"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="dashDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="334" name="꺾인 연결선 333"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="324" idx="2"/>
+            <a:endCxn id="318" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="3458135" y="42683207"/>
+            <a:ext cx="869578" cy="2514599"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 42784"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="dashDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -13591,62 +16892,89 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </a:spPr>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:AF87"/>
+  <dimension ref="D2:BD190"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A104" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ137" sqref="AJ137"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F175" sqref="F175"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="2" defaultRowHeight="19.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="2" style="9"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D2" s="2" t="s">
+    <row r="2" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="3" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D3" t="s">
+    <row r="3" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="9" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D4" t="s">
+    <row r="4" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="9" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="4:9" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="4:9" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="D23" s="7" t="s">
+    <row r="23" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="57" spans="5:12" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="58" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="58" spans="5:12" x14ac:dyDescent="0.25">
       <c r="L58" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="60" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="60" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E60" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="61" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="61" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E61" s="2" t="s">
         <v>155</v>
       </c>
@@ -13654,7 +16982,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="62" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="62" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E62" s="2" t="s">
         <v>156</v>
       </c>
@@ -13662,12 +16990,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="63" spans="5:12" x14ac:dyDescent="0.2">
+    <row r="63" spans="5:12" x14ac:dyDescent="0.25">
       <c r="L63" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="65" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="65" spans="5:32" x14ac:dyDescent="0.25">
       <c r="E65" s="2" t="s">
         <v>157</v>
       </c>
@@ -13675,7 +17003,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="66" spans="5:32" x14ac:dyDescent="0.25">
       <c r="E66" s="2" t="s">
         <v>158</v>
       </c>
@@ -13683,7 +17011,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="67" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="67" spans="5:32" x14ac:dyDescent="0.25">
       <c r="E67" s="2" t="s">
         <v>160</v>
       </c>
@@ -13691,17 +17019,17 @@
         <v>161</v>
       </c>
     </row>
-    <row r="68" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="68" spans="5:32" x14ac:dyDescent="0.25">
       <c r="L68" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="70" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="70" spans="5:32" x14ac:dyDescent="0.25">
       <c r="E70" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="71" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="71" spans="5:32" x14ac:dyDescent="0.25">
       <c r="E71" s="2" t="s">
         <v>164</v>
       </c>
@@ -13709,7 +17037,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="72" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="72" spans="5:32" x14ac:dyDescent="0.25">
       <c r="E72" s="2" t="s">
         <v>166</v>
       </c>
@@ -13717,7 +17045,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="73" spans="5:32" x14ac:dyDescent="0.25">
       <c r="E73" s="2" t="s">
         <v>168</v>
       </c>
@@ -13725,17 +17053,17 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="74" spans="5:32" x14ac:dyDescent="0.25">
       <c r="I74" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="76" spans="5:32" x14ac:dyDescent="0.25">
       <c r="E76" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="78" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="78" spans="5:32" x14ac:dyDescent="0.25">
       <c r="E78" s="2" t="s">
         <v>172</v>
       </c>
@@ -13743,17 +17071,17 @@
         <v>173</v>
       </c>
     </row>
-    <row r="79" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="79" spans="5:32" x14ac:dyDescent="0.25">
       <c r="N79" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="80" spans="5:32" x14ac:dyDescent="0.2">
+    <row r="80" spans="5:32" x14ac:dyDescent="0.25">
       <c r="Z80" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="82" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="82" spans="4:12" x14ac:dyDescent="0.25">
       <c r="E82" s="2" t="s">
         <v>175</v>
       </c>
@@ -13761,14 +17089,196 @@
         <v>176</v>
       </c>
     </row>
-    <row r="83" spans="4:12" x14ac:dyDescent="0.2">
+    <row r="83" spans="4:12" x14ac:dyDescent="0.25">
       <c r="L83" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="87" spans="4:12" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="D87" s="7" t="s">
+    <row r="87" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D87" s="4" t="s">
         <v>181</v>
+      </c>
+    </row>
+    <row r="132" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D132" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="133" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="134" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E134" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="136" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E136" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="137" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E137" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="138" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H138" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="139" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E139" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="140" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H140" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="141" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E141" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="142" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="E142" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="143" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H143" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="144" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H144" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="145" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="H145" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="147" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="D147" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="148" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="E148" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="153" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="T153" t="s">
+        <v>199</v>
+      </c>
+      <c r="AN153" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="156" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="AO156" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="158" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="AN158" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="160" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="AN160" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="161" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="AP161" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="163" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="I163" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ163" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="165" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="D165" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="166" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="E166" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="168" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="D168" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="169" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="E169" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="171" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="E171" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="172" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="F172" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="173" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="F173" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="174" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="F174" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="180" spans="5:56" x14ac:dyDescent="0.25">
+      <c r="K180" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="185" spans="5:56" x14ac:dyDescent="0.25">
+      <c r="AV185" t="s">
+        <v>216</v>
+      </c>
+      <c r="BD185" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="186" spans="5:56" x14ac:dyDescent="0.25">
+      <c r="AV186" t="s">
+        <v>217</v>
+      </c>
+      <c r="BD186" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="188" spans="5:56" x14ac:dyDescent="0.25">
+      <c r="R188" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="190" spans="5:56" x14ac:dyDescent="0.25">
+      <c r="E190" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -13781,10 +17291,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:AH173"/>
+  <dimension ref="D2:AH176"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AU170" sqref="AU170"/>
+    <sheetView showGridLines="0" topLeftCell="A124" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J101" sqref="J101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2" defaultRowHeight="16.2" x14ac:dyDescent="0.2"/>
@@ -14086,232 +17596,232 @@
       </c>
     </row>
     <row r="78" spans="6:34" ht="16.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G78" s="5" t="s">
+      <c r="G78" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
-      <c r="J78" s="5"/>
-      <c r="K78" s="5"/>
-      <c r="L78" s="5"/>
-      <c r="M78" s="5"/>
-      <c r="N78" s="5" t="s">
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="6"/>
+      <c r="N78" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="O78" s="5"/>
-      <c r="P78" s="5"/>
-      <c r="Q78" s="5"/>
-      <c r="R78" s="5"/>
-      <c r="S78" s="5"/>
-      <c r="T78" s="5" t="s">
+      <c r="O78" s="6"/>
+      <c r="P78" s="6"/>
+      <c r="Q78" s="6"/>
+      <c r="R78" s="6"/>
+      <c r="S78" s="6"/>
+      <c r="T78" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="U78" s="5"/>
-      <c r="V78" s="5"/>
-      <c r="W78" s="5"/>
-      <c r="X78" s="5"/>
-      <c r="Y78" s="5"/>
-      <c r="Z78" s="5" t="s">
+      <c r="U78" s="6"/>
+      <c r="V78" s="6"/>
+      <c r="W78" s="6"/>
+      <c r="X78" s="6"/>
+      <c r="Y78" s="6"/>
+      <c r="Z78" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="AA78" s="5"/>
-      <c r="AB78" s="5"/>
-      <c r="AC78" s="5"/>
-      <c r="AD78" s="5"/>
-      <c r="AE78" s="5"/>
-      <c r="AF78" s="5"/>
-      <c r="AG78" s="5"/>
-      <c r="AH78" s="5"/>
+      <c r="AA78" s="6"/>
+      <c r="AB78" s="6"/>
+      <c r="AC78" s="6"/>
+      <c r="AD78" s="6"/>
+      <c r="AE78" s="6"/>
+      <c r="AF78" s="6"/>
+      <c r="AG78" s="6"/>
+      <c r="AH78" s="6"/>
     </row>
     <row r="79" spans="6:34" ht="16.8" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="G79" s="6" t="s">
+      <c r="G79" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="6"/>
-      <c r="L79" s="6"/>
-      <c r="M79" s="6"/>
-      <c r="N79" s="6" t="s">
+      <c r="H79" s="7"/>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="7"/>
+      <c r="N79" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="O79" s="6"/>
-      <c r="P79" s="6"/>
-      <c r="Q79" s="6"/>
-      <c r="R79" s="6"/>
-      <c r="S79" s="6"/>
-      <c r="T79" s="6" t="s">
+      <c r="O79" s="7"/>
+      <c r="P79" s="7"/>
+      <c r="Q79" s="7"/>
+      <c r="R79" s="7"/>
+      <c r="S79" s="7"/>
+      <c r="T79" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="U79" s="6"/>
-      <c r="V79" s="6"/>
-      <c r="W79" s="6"/>
-      <c r="X79" s="6"/>
-      <c r="Y79" s="6"/>
-      <c r="Z79" s="6" t="s">
+      <c r="U79" s="7"/>
+      <c r="V79" s="7"/>
+      <c r="W79" s="7"/>
+      <c r="X79" s="7"/>
+      <c r="Y79" s="7"/>
+      <c r="Z79" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="AA79" s="6"/>
-      <c r="AB79" s="6"/>
-      <c r="AC79" s="6"/>
-      <c r="AD79" s="6"/>
-      <c r="AE79" s="6"/>
-      <c r="AF79" s="6"/>
-      <c r="AG79" s="6"/>
-      <c r="AH79" s="6"/>
+      <c r="AA79" s="7"/>
+      <c r="AB79" s="7"/>
+      <c r="AC79" s="7"/>
+      <c r="AD79" s="7"/>
+      <c r="AE79" s="7"/>
+      <c r="AF79" s="7"/>
+      <c r="AG79" s="7"/>
+      <c r="AH79" s="7"/>
     </row>
     <row r="80" spans="6:34" x14ac:dyDescent="0.2">
-      <c r="G80" s="4" t="s">
+      <c r="G80" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-      <c r="J80" s="4"/>
-      <c r="K80" s="4"/>
-      <c r="L80" s="4"/>
-      <c r="M80" s="4"/>
-      <c r="N80" s="4" t="s">
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+      <c r="J80" s="5"/>
+      <c r="K80" s="5"/>
+      <c r="L80" s="5"/>
+      <c r="M80" s="5"/>
+      <c r="N80" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="O80" s="4"/>
-      <c r="P80" s="4"/>
-      <c r="Q80" s="4"/>
-      <c r="R80" s="4"/>
-      <c r="S80" s="4"/>
-      <c r="T80" s="4" t="s">
+      <c r="O80" s="5"/>
+      <c r="P80" s="5"/>
+      <c r="Q80" s="5"/>
+      <c r="R80" s="5"/>
+      <c r="S80" s="5"/>
+      <c r="T80" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="U80" s="4"/>
-      <c r="V80" s="4"/>
-      <c r="W80" s="4"/>
-      <c r="X80" s="4"/>
-      <c r="Y80" s="4"/>
-      <c r="Z80" s="4" t="s">
+      <c r="U80" s="5"/>
+      <c r="V80" s="5"/>
+      <c r="W80" s="5"/>
+      <c r="X80" s="5"/>
+      <c r="Y80" s="5"/>
+      <c r="Z80" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AA80" s="4"/>
-      <c r="AB80" s="4"/>
-      <c r="AC80" s="4"/>
-      <c r="AD80" s="4"/>
-      <c r="AE80" s="4"/>
-      <c r="AF80" s="4"/>
-      <c r="AG80" s="4"/>
-      <c r="AH80" s="4"/>
+      <c r="AA80" s="5"/>
+      <c r="AB80" s="5"/>
+      <c r="AC80" s="5"/>
+      <c r="AD80" s="5"/>
+      <c r="AE80" s="5"/>
+      <c r="AF80" s="5"/>
+      <c r="AG80" s="5"/>
+      <c r="AH80" s="5"/>
     </row>
     <row r="81" spans="4:34" x14ac:dyDescent="0.2">
-      <c r="G81" s="4" t="s">
+      <c r="G81" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
-      <c r="K81" s="4"/>
-      <c r="L81" s="4"/>
-      <c r="M81" s="4"/>
-      <c r="N81" s="4" t="s">
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+      <c r="J81" s="5"/>
+      <c r="K81" s="5"/>
+      <c r="L81" s="5"/>
+      <c r="M81" s="5"/>
+      <c r="N81" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O81" s="4"/>
-      <c r="P81" s="4"/>
-      <c r="Q81" s="4"/>
-      <c r="R81" s="4"/>
-      <c r="S81" s="4"/>
-      <c r="T81" s="4" t="s">
+      <c r="O81" s="5"/>
+      <c r="P81" s="5"/>
+      <c r="Q81" s="5"/>
+      <c r="R81" s="5"/>
+      <c r="S81" s="5"/>
+      <c r="T81" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="U81" s="4"/>
-      <c r="V81" s="4"/>
-      <c r="W81" s="4"/>
-      <c r="X81" s="4"/>
-      <c r="Y81" s="4"/>
-      <c r="Z81" s="4" t="s">
+      <c r="U81" s="5"/>
+      <c r="V81" s="5"/>
+      <c r="W81" s="5"/>
+      <c r="X81" s="5"/>
+      <c r="Y81" s="5"/>
+      <c r="Z81" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AA81" s="4"/>
-      <c r="AB81" s="4"/>
-      <c r="AC81" s="4"/>
-      <c r="AD81" s="4"/>
-      <c r="AE81" s="4"/>
-      <c r="AF81" s="4"/>
-      <c r="AG81" s="4"/>
-      <c r="AH81" s="4"/>
+      <c r="AA81" s="5"/>
+      <c r="AB81" s="5"/>
+      <c r="AC81" s="5"/>
+      <c r="AD81" s="5"/>
+      <c r="AE81" s="5"/>
+      <c r="AF81" s="5"/>
+      <c r="AG81" s="5"/>
+      <c r="AH81" s="5"/>
     </row>
     <row r="82" spans="4:34" x14ac:dyDescent="0.2">
-      <c r="G82" s="4" t="s">
+      <c r="G82" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-      <c r="J82" s="4"/>
-      <c r="K82" s="4"/>
-      <c r="L82" s="4"/>
-      <c r="M82" s="4"/>
-      <c r="N82" s="4" t="s">
+      <c r="H82" s="5"/>
+      <c r="I82" s="5"/>
+      <c r="J82" s="5"/>
+      <c r="K82" s="5"/>
+      <c r="L82" s="5"/>
+      <c r="M82" s="5"/>
+      <c r="N82" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="O82" s="4"/>
-      <c r="P82" s="4"/>
-      <c r="Q82" s="4"/>
-      <c r="R82" s="4"/>
-      <c r="S82" s="4"/>
-      <c r="T82" s="4" t="s">
+      <c r="O82" s="5"/>
+      <c r="P82" s="5"/>
+      <c r="Q82" s="5"/>
+      <c r="R82" s="5"/>
+      <c r="S82" s="5"/>
+      <c r="T82" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="U82" s="4"/>
-      <c r="V82" s="4"/>
-      <c r="W82" s="4"/>
-      <c r="X82" s="4"/>
-      <c r="Y82" s="4"/>
-      <c r="Z82" s="4" t="s">
+      <c r="U82" s="5"/>
+      <c r="V82" s="5"/>
+      <c r="W82" s="5"/>
+      <c r="X82" s="5"/>
+      <c r="Y82" s="5"/>
+      <c r="Z82" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="AA82" s="4"/>
-      <c r="AB82" s="4"/>
-      <c r="AC82" s="4"/>
-      <c r="AD82" s="4"/>
-      <c r="AE82" s="4"/>
-      <c r="AF82" s="4"/>
-      <c r="AG82" s="4"/>
-      <c r="AH82" s="4"/>
+      <c r="AA82" s="5"/>
+      <c r="AB82" s="5"/>
+      <c r="AC82" s="5"/>
+      <c r="AD82" s="5"/>
+      <c r="AE82" s="5"/>
+      <c r="AF82" s="5"/>
+      <c r="AG82" s="5"/>
+      <c r="AH82" s="5"/>
     </row>
     <row r="83" spans="4:34" x14ac:dyDescent="0.2">
-      <c r="G83" s="4" t="s">
+      <c r="G83" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-      <c r="J83" s="4"/>
-      <c r="K83" s="4"/>
-      <c r="L83" s="4"/>
-      <c r="M83" s="4"/>
-      <c r="N83" s="4" t="s">
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+      <c r="J83" s="5"/>
+      <c r="K83" s="5"/>
+      <c r="L83" s="5"/>
+      <c r="M83" s="5"/>
+      <c r="N83" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="O83" s="4"/>
-      <c r="P83" s="4"/>
-      <c r="Q83" s="4"/>
-      <c r="R83" s="4"/>
-      <c r="S83" s="4"/>
-      <c r="T83" s="4" t="s">
+      <c r="O83" s="5"/>
+      <c r="P83" s="5"/>
+      <c r="Q83" s="5"/>
+      <c r="R83" s="5"/>
+      <c r="S83" s="5"/>
+      <c r="T83" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="U83" s="4"/>
-      <c r="V83" s="4"/>
-      <c r="W83" s="4"/>
-      <c r="X83" s="4"/>
-      <c r="Y83" s="4"/>
-      <c r="Z83" s="4" t="s">
+      <c r="U83" s="5"/>
+      <c r="V83" s="5"/>
+      <c r="W83" s="5"/>
+      <c r="X83" s="5"/>
+      <c r="Y83" s="5"/>
+      <c r="Z83" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AA83" s="4"/>
-      <c r="AB83" s="4"/>
-      <c r="AC83" s="4"/>
-      <c r="AD83" s="4"/>
-      <c r="AE83" s="4"/>
-      <c r="AF83" s="4"/>
-      <c r="AG83" s="4"/>
-      <c r="AH83" s="4"/>
+      <c r="AA83" s="5"/>
+      <c r="AB83" s="5"/>
+      <c r="AC83" s="5"/>
+      <c r="AD83" s="5"/>
+      <c r="AE83" s="5"/>
+      <c r="AF83" s="5"/>
+      <c r="AG83" s="5"/>
+      <c r="AH83" s="5"/>
     </row>
     <row r="85" spans="4:34" x14ac:dyDescent="0.2">
       <c r="D85" s="1" t="s">
@@ -14382,243 +17892,266 @@
         <v>84</v>
       </c>
     </row>
-    <row r="102" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D102" s="1" t="s">
+    <row r="101" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="F101" s="3"/>
+      <c r="G101" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="103" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D103" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="104" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="E104" s="2" t="s">
+    <row r="105" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="E105" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="105" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="F105" t="s">
+    <row r="106" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="F106" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="E107" s="2" t="s">
+    <row r="108" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="E108" s="2" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="109" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="F109" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="110" spans="4:18" x14ac:dyDescent="0.2">
       <c r="F110" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="111" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="F111" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="112" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="F112" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="113" spans="4:6" x14ac:dyDescent="0.2">
       <c r="F113" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="114" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F114" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="115" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D115" s="1" t="s">
+    <row r="116" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D116" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="117" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E117" s="2" t="s">
+    <row r="118" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E118" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="118" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F118" t="s">
+    <row r="119" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F119" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="120" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E120" s="2" t="s">
+    <row r="121" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E121" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="121" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F121" t="s">
+    <row r="122" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F122" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="124" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D124" s="1" t="s">
+    <row r="125" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D125" s="1" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="126" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E126" s="2" t="s">
+    <row r="127" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E127" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="127" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F127" s="3" t="s">
+    <row r="128" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F128" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="128" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F128" t="s">
+    <row r="129" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="F129" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="129" spans="5:16" x14ac:dyDescent="0.2">
-      <c r="P129" t="s">
+    <row r="130" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="P130" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="131" spans="5:16" x14ac:dyDescent="0.2">
-      <c r="E131" s="2" t="s">
+    <row r="132" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E132" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="132" spans="5:16" x14ac:dyDescent="0.2">
-      <c r="F132" t="s">
+    <row r="133" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="F133" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="134" spans="5:16" x14ac:dyDescent="0.2">
-      <c r="F134" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="135" spans="5:16" x14ac:dyDescent="0.2">
       <c r="F135" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="136" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="F136" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="137" spans="5:16" x14ac:dyDescent="0.2">
-      <c r="F137" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="138" spans="5:16" x14ac:dyDescent="0.2">
       <c r="F138" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="139" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="F139" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="140" spans="5:16" x14ac:dyDescent="0.2">
-      <c r="E140" s="2" t="s">
+    <row r="141" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E141" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="141" spans="5:16" x14ac:dyDescent="0.2">
-      <c r="F141" t="s">
+    <row r="142" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="F142" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="142" spans="5:16" x14ac:dyDescent="0.2">
-      <c r="G142" t="s">
+    <row r="143" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="G143" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="144" spans="5:16" x14ac:dyDescent="0.2">
-      <c r="F144" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="145" spans="4:8" x14ac:dyDescent="0.2">
       <c r="F145" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="146" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F146" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="148" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="D148" s="1" t="s">
+    <row r="149" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="D149" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="150" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="E150" s="2" t="s">
+    <row r="151" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E151" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="151" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="F151" t="s">
+    <row r="152" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F152" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="153" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="E153" s="2" t="s">
+    <row r="154" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E154" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="154" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="F154" t="s">
+    <row r="155" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F155" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="155" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="G155" t="s">
+    <row r="156" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="G156" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="156" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="H156" t="s">
+    <row r="157" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="H157" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="158" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="E158" s="2" t="s">
+    <row r="159" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="E159" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="159" spans="4:8" x14ac:dyDescent="0.2">
-      <c r="F159" t="s">
+    <row r="160" spans="4:8" x14ac:dyDescent="0.2">
+      <c r="F160" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="161" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D161" s="1" t="s">
+    <row r="162" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D162" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="163" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E163" s="2" t="s">
+    <row r="164" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E164" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="164" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F164" t="s">
+    <row r="165" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F165" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="166" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E166" s="2" t="s">
+    <row r="167" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E167" s="2" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="167" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F167" t="s">
+    <row r="168" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F168" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="169" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E169" s="2" t="s">
+    <row r="170" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E170" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="170" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F170" t="s">
+    <row r="171" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F171" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="172" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E172" s="2" t="s">
+    <row r="173" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E173" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="173" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="F173" t="s">
+    <row r="174" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="F174" t="s">
         <v>145</v>
+      </c>
+    </row>
+    <row r="176" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D176" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="N83:S83"/>
+    <mergeCell ref="G78:M78"/>
+    <mergeCell ref="G79:M79"/>
+    <mergeCell ref="G80:M80"/>
+    <mergeCell ref="G81:M81"/>
+    <mergeCell ref="G82:M82"/>
+    <mergeCell ref="G83:M83"/>
+    <mergeCell ref="N78:S78"/>
+    <mergeCell ref="N79:S79"/>
+    <mergeCell ref="N80:S80"/>
+    <mergeCell ref="N81:S81"/>
+    <mergeCell ref="N82:S82"/>
     <mergeCell ref="Z83:AH83"/>
     <mergeCell ref="T78:Y78"/>
     <mergeCell ref="T79:Y79"/>
@@ -14631,18 +18164,6 @@
     <mergeCell ref="Z80:AH80"/>
     <mergeCell ref="Z81:AH81"/>
     <mergeCell ref="Z82:AH82"/>
-    <mergeCell ref="N83:S83"/>
-    <mergeCell ref="G78:M78"/>
-    <mergeCell ref="G79:M79"/>
-    <mergeCell ref="G80:M80"/>
-    <mergeCell ref="G81:M81"/>
-    <mergeCell ref="G82:M82"/>
-    <mergeCell ref="G83:M83"/>
-    <mergeCell ref="N78:S78"/>
-    <mergeCell ref="N79:S79"/>
-    <mergeCell ref="N80:S80"/>
-    <mergeCell ref="N81:S81"/>
-    <mergeCell ref="N82:S82"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20220120 update kubernetes document
・Added about Ingress
</commit_message>
<xml_diff>
--- a/Kubernetes.xlsx
+++ b/Kubernetes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="241">
   <si>
     <t>node&amp;pod確認</t>
     <rPh sb="8" eb="10">
@@ -2311,12 +2311,308 @@
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>複数Deployment、複数NodePortが必要な場合使用</t>
+    <rPh sb="0" eb="2">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>バアイ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>固有な住所を提供し、使用目的によって異なるResponseが提供できるし、Trafficに対する L4/L7 LoadBalancerと保安証明書を処理機能を提供</t>
+    <rPh sb="0" eb="2">
+      <t>コユウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジュウショ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>モクテキ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>テイキョウ</t>
+    </rPh>
+    <rPh sb="45" eb="46">
+      <t>タイ</t>
+    </rPh>
+    <rPh sb="68" eb="70">
+      <t>ホアン</t>
+    </rPh>
+    <rPh sb="70" eb="73">
+      <t>ショウメイショ</t>
+    </rPh>
+    <rPh sb="74" eb="76">
+      <t>ショリ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>キノウ</t>
+    </rPh>
+    <rPh sb="79" eb="81">
+      <t>テイキョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※IngressするためにはIngressControllerが必要</t>
+    <rPh sb="32" eb="34">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>　IngressControllerは、直接Podと通信できないためNodePortまたはLoadBalancer Serviceと連動する必要がある</t>
+    <rPh sb="20" eb="22">
+      <t>チョクセツ</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ツウシン</t>
+    </rPh>
+    <rPh sb="66" eb="68">
+      <t>レンドウ</t>
+    </rPh>
+    <rPh sb="70" eb="72">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>①UserはNodeごとに設定されたNodePortを通してNodePort serviceにアクセスする。</t>
+    <rPh sb="13" eb="15">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>トオ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>②IngressControllerはUserの接続経路に従って適切なClusterIP Serviceで経路を提供する</t>
+    <rPh sb="24" eb="26">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="26" eb="28">
+      <t>ケイロ</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>シタガ</t>
+    </rPh>
+    <rPh sb="32" eb="34">
+      <t>テキセツ</t>
+    </rPh>
+    <rPh sb="53" eb="55">
+      <t>ケイロ</t>
+    </rPh>
+    <rPh sb="56" eb="58">
+      <t>テイキョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>③ClusterIP ServiceはUserを対象Podに連携する</t>
+    <rPh sb="24" eb="26">
+      <t>タイショウ</t>
+    </rPh>
+    <rPh sb="30" eb="32">
+      <t>レンケイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>http://hostname:30100/</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>http://hostname:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ip</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-&gt; 80portのip podへ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-&gt; 80portのhname podへ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>http</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>://hostname:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30101</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/ip</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>http</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>://hostname:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>30101</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-&gt; 443portのhname podへ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-&gt; 443portのip podへ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>pathでどのServiceにつなげるか指定可能</t>
+    <rPh sb="20" eb="22">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>カノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数のportも指定可能</t>
+    <rPh sb="0" eb="2">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>シテイ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>カノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LoadBalancer</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2398,6 +2694,13 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2474,11 +2777,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -15518,7 +15821,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Worker Node #1</a:t>
+              <a:t>Worker Node #2</a:t>
             </a:r>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
               <a:solidFill>
@@ -15592,7 +15895,7 @@
                   <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
               </a:rPr>
-              <a:t>Worker Node #1</a:t>
+              <a:t>Worker Node #3</a:t>
             </a:r>
             <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
               <a:solidFill>
@@ -16606,6 +16909,2392 @@
           </a:fontRef>
         </xdr:style>
       </xdr:cxnSp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>199</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>98612</xdr:colOff>
+      <xdr:row>216</xdr:row>
+      <xdr:rowOff>242046</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="453" name="그룹 452"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="672352" y="48167365"/>
+          <a:ext cx="7763436" cy="4356846"/>
+          <a:chOff x="672352" y="48167365"/>
+          <a:chExt cx="7763436" cy="4356846"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="252" name="직사각형 251"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="672352" y="49252094"/>
+            <a:ext cx="7763436" cy="941295"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>NodePort Service</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="254" name="직사각형 253"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="672352" y="50211318"/>
+            <a:ext cx="7736542" cy="2312893"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="60000"/>
+              <a:lumOff val="40000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="267" name="직사각형 266"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="770965" y="51367764"/>
+            <a:ext cx="2321859" cy="1066799"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Port(80:30100/TCP)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Port(443:30101/TCP)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Worker Node #1</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="278" name="직사각형 277"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3334872" y="51367764"/>
+            <a:ext cx="2330824" cy="1066799"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Port(80:30000/TCP)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Port(443:30101/TCP)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Worker Node #2</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="279" name="직사각형 278"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5827059" y="51367764"/>
+            <a:ext cx="2312894" cy="1066799"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Port(80:30000/TCP)</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Port(443:30101/TCP)</a:t>
+            </a:r>
+            <a:endParaRPr lang="ja-JP" altLang="ja-JP">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Worker Node #3</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:grpSp>
+        <xdr:nvGrpSpPr>
+          <xdr:cNvPr id="281" name="그룹 280"/>
+          <xdr:cNvGrpSpPr/>
+        </xdr:nvGrpSpPr>
+        <xdr:grpSpPr>
+          <a:xfrm>
+            <a:off x="851649" y="48167365"/>
+            <a:ext cx="526452" cy="959223"/>
+            <a:chOff x="1210235" y="16324729"/>
+            <a:chExt cx="526452" cy="851647"/>
+          </a:xfrm>
+        </xdr:grpSpPr>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="304" name="순서도: 지연 303"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm rot="16200000">
+              <a:off x="1284081" y="16750441"/>
+              <a:ext cx="352089" cy="499782"/>
+            </a:xfrm>
+            <a:prstGeom prst="flowChartDelay">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="305" name="타원 304"/>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1272315" y="16517918"/>
+              <a:ext cx="388172" cy="371139"/>
+            </a:xfrm>
+            <a:prstGeom prst="ellipse">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:sysClr val="window" lastClr="FFFFFF"/>
+            </a:solidFill>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="2">
+              <a:schemeClr val="accent1">
+                <a:shade val="50000"/>
+              </a:schemeClr>
+            </a:lnRef>
+            <a:fillRef idx="1">
+              <a:schemeClr val="accent1"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:schemeClr val="accent1"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="lt1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr algn="l"/>
+              <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="306" name="TextBox 305"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="1244525" y="16324729"/>
+              <a:ext cx="492162" cy="216049"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525" cmpd="sng">
+              <a:noFill/>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="dk1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                </a:rPr>
+                <a:t>User</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </xdr:grpSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="282" name="꺾인 연결선 281"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="304" idx="1"/>
+            <a:endCxn id="291" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="-123821" y="50133436"/>
+            <a:ext cx="2232209" cy="218515"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 82128"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="284" name="꺾인 연결선 283"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="304" idx="1"/>
+            <a:endCxn id="292" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="1171578" y="49056550"/>
+            <a:ext cx="2250138" cy="2390215"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 80677"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="285" name="꺾인 연결선 284"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="304" idx="1"/>
+            <a:endCxn id="293" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="2408709" y="47819420"/>
+            <a:ext cx="2232209" cy="4846546"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 81727"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="286" name="TextBox 285"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1093696" y="49287953"/>
+            <a:ext cx="325730" cy="275717"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+              <a:t>①</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="287" name="꺾인 연결선 286"/>
+          <xdr:cNvCxnSpPr>
+            <a:endCxn id="385" idx="4"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000" flipH="1" flipV="1">
+            <a:off x="1454524" y="50630421"/>
+            <a:ext cx="1201272" cy="219631"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 25373"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="291" name="타원 290"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="788896" y="51358798"/>
+            <a:ext cx="188258" cy="206188"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="292" name="타원 291"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3397626" y="51376727"/>
+            <a:ext cx="188258" cy="206188"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="293" name="타원 292"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5853957" y="51358798"/>
+            <a:ext cx="188258" cy="206188"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="294" name="꺾인 연결선 293"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="278" idx="0"/>
+            <a:endCxn id="385" idx="4"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipV="1">
+            <a:off x="2718548" y="49586028"/>
+            <a:ext cx="1228164" cy="2335308"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 26642"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="295" name="꺾인 연결선 294"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="279" idx="0"/>
+            <a:endCxn id="385" idx="4"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipV="1">
+            <a:off x="3960159" y="48344417"/>
+            <a:ext cx="1228164" cy="4818530"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 27372"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="296" name="TextBox 295"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1649507" y="51089858"/>
+            <a:ext cx="325730" cy="275717"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>②</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="297" name="직사각형 296"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2079809" y="51609812"/>
+            <a:ext cx="941297" cy="376518"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>POD(hname)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="300" name="꺾인 연결선 299"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="371" idx="2"/>
+            <a:endCxn id="406" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="5125571" y="48846441"/>
+            <a:ext cx="1102659" cy="4800600"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector4">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 41463"/>
+              <a:gd name="adj2" fmla="val 104762"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="dashDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="302" name="꺾인 연결선 301"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="371" idx="2"/>
+            <a:endCxn id="400" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="3861547" y="50110464"/>
+            <a:ext cx="1102659" cy="2272553"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector4">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 41463"/>
+              <a:gd name="adj2" fmla="val 110059"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="dashDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="303" name="꺾인 연결선 302"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="371" idx="2"/>
+            <a:endCxn id="297" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="2597524" y="51118994"/>
+            <a:ext cx="1102659" cy="255494"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector2">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:prstDash val="dashDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="353" name="직사각형 352"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2599765" y="49512071"/>
+            <a:ext cx="1353670" cy="502023"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>hname-svc</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>&lt;path: /&gt;</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="354" name="직사각형 353"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4347883" y="49521036"/>
+            <a:ext cx="1353670" cy="502023"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>ip-svc</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>&lt;path: /ip&gt;</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="361" name="직사각형 360"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2079809" y="52022188"/>
+            <a:ext cx="941297" cy="376518"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>POD(ip)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="371" name="직사각형 370"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2599765" y="50238212"/>
+            <a:ext cx="1353670" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>ClusterIP Service</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>(hname-svc)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="372" name="직사각형 371"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4347883" y="50238212"/>
+            <a:ext cx="1353670" cy="457200"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="20000"/>
+                <a:lumOff val="80000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>ClusterIP Service</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>(ip-svc)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="385" name="타원 384"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2070847" y="49933412"/>
+            <a:ext cx="188258" cy="206188"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="95000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="400" name="직사각형 399"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4607856" y="51609812"/>
+            <a:ext cx="941297" cy="376518"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>POD(hname)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="401" name="직사각형 400"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="4607856" y="52022188"/>
+            <a:ext cx="941297" cy="376518"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>POD(ip)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="406" name="직사각형 405"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7135903" y="51609812"/>
+            <a:ext cx="941297" cy="376518"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>POD(hname)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="407" name="직사각형 406"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="7135903" y="52022188"/>
+            <a:ext cx="941297" cy="376518"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg1">
+              <a:lumMod val="65000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="bg1">
+                <a:lumMod val="65000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>POD(ip)</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="419" name="꺾인 연결선 418"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="372" idx="2"/>
+            <a:endCxn id="361" idx="2"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="5400000">
+            <a:off x="2935941" y="50309929"/>
+            <a:ext cx="1703294" cy="2474260"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector3">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 33421"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:prstDash val="dashDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="429" name="꺾인 연결선 428"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="372" idx="2"/>
+            <a:endCxn id="401" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="4529418" y="51190711"/>
+            <a:ext cx="1515035" cy="524435"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector4">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 37278"/>
+              <a:gd name="adj2" fmla="val 131624"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:prstDash val="dashDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="435" name="꺾인 연결선 434"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="372" idx="2"/>
+            <a:endCxn id="407" idx="3"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000" flipH="1">
+            <a:off x="5793442" y="49926688"/>
+            <a:ext cx="1515035" cy="3052482"/>
+          </a:xfrm>
+          <a:prstGeom prst="bentConnector4">
+            <a:avLst>
+              <a:gd name="adj1" fmla="val 36686"/>
+              <a:gd name="adj2" fmla="val 107489"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:prstDash val="dashDot"/>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="442" name="직선 화살표 연결선 441"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="353" idx="2"/>
+            <a:endCxn id="371" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3276600" y="50014094"/>
+            <a:ext cx="0" cy="224118"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="15875">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="446" name="직선 화살표 연결선 445"/>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="354" idx="2"/>
+            <a:endCxn id="372" idx="0"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5024718" y="50023059"/>
+            <a:ext cx="0" cy="215153"/>
+          </a:xfrm>
+          <a:prstGeom prst="straightConnector1">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:ln w="15875">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:tailEnd type="triangle"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="449" name="TextBox 448"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3307976" y="50005130"/>
+            <a:ext cx="325730" cy="275717"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>③</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="450" name="TextBox 449"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5074023" y="50005130"/>
+            <a:ext cx="325730" cy="275717"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>③</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="451" name="TextBox 450"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3281082" y="50704376"/>
+            <a:ext cx="325730" cy="275717"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>④</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="452" name="TextBox 451"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5020235" y="50704376"/>
+            <a:ext cx="325730" cy="275717"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:noAutofit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>④</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
@@ -16923,29 +19612,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:BD190"/>
+  <dimension ref="D2:BM220"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F175" sqref="F175"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A220" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="CE205" sqref="CE205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2" defaultRowHeight="19.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="2" style="9"/>
+    <col min="4" max="4" width="2" style="6"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="5" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="3" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="6" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="4" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="6" t="s">
         <v>148</v>
       </c>
     </row>
@@ -17100,7 +19789,7 @@
       </c>
     </row>
     <row r="132" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D132" s="9" t="s">
+      <c r="D132" s="6" t="s">
         <v>184</v>
       </c>
     </row>
@@ -17165,7 +19854,7 @@
       </c>
     </row>
     <row r="147" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="D147" s="9" t="s">
+      <c r="D147" s="6" t="s">
         <v>197</v>
       </c>
     </row>
@@ -17211,7 +19900,7 @@
       </c>
     </row>
     <row r="165" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="D165" s="9" t="s">
+      <c r="D165" s="6" t="s">
         <v>202</v>
       </c>
     </row>
@@ -17221,7 +19910,7 @@
       </c>
     </row>
     <row r="168" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="D168" s="9" t="s">
+      <c r="D168" s="6" t="s">
         <v>210</v>
       </c>
     </row>
@@ -17279,6 +19968,84 @@
     <row r="190" spans="5:56" x14ac:dyDescent="0.25">
       <c r="E190" s="2" t="s">
         <v>221</v>
+      </c>
+    </row>
+    <row r="191" spans="5:56" x14ac:dyDescent="0.25">
+      <c r="F191" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="192" spans="5:56" x14ac:dyDescent="0.25">
+      <c r="F192" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="193" spans="6:54" x14ac:dyDescent="0.25">
+      <c r="F193" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="194" spans="6:54" x14ac:dyDescent="0.25">
+      <c r="F194" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="196" spans="6:54" x14ac:dyDescent="0.25">
+      <c r="F196" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="197" spans="6:54" x14ac:dyDescent="0.25">
+      <c r="F197" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="198" spans="6:54" x14ac:dyDescent="0.25">
+      <c r="F198" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="201" spans="6:54" x14ac:dyDescent="0.25">
+      <c r="N201" t="s">
+        <v>230</v>
+      </c>
+      <c r="AA201" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="AO201" t="s">
+        <v>235</v>
+      </c>
+      <c r="BB201" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="202" spans="6:54" x14ac:dyDescent="0.25">
+      <c r="N202" t="s">
+        <v>231</v>
+      </c>
+      <c r="AA202" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="AO202" t="s">
+        <v>234</v>
+      </c>
+      <c r="BB202" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="209" spans="5:65" x14ac:dyDescent="0.25">
+      <c r="BM209" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="210" spans="5:65" x14ac:dyDescent="0.25">
+      <c r="BM210" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="220" spans="5:65" x14ac:dyDescent="0.25">
+      <c r="E220" s="2" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -17596,232 +20363,232 @@
       </c>
     </row>
     <row r="78" spans="6:34" ht="16.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G78" s="6" t="s">
+      <c r="G78" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="6"/>
-      <c r="L78" s="6"/>
-      <c r="M78" s="6"/>
-      <c r="N78" s="6" t="s">
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+      <c r="K78" s="8"/>
+      <c r="L78" s="8"/>
+      <c r="M78" s="8"/>
+      <c r="N78" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="O78" s="6"/>
-      <c r="P78" s="6"/>
-      <c r="Q78" s="6"/>
-      <c r="R78" s="6"/>
-      <c r="S78" s="6"/>
-      <c r="T78" s="6" t="s">
+      <c r="O78" s="8"/>
+      <c r="P78" s="8"/>
+      <c r="Q78" s="8"/>
+      <c r="R78" s="8"/>
+      <c r="S78" s="8"/>
+      <c r="T78" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="U78" s="6"/>
-      <c r="V78" s="6"/>
-      <c r="W78" s="6"/>
-      <c r="X78" s="6"/>
-      <c r="Y78" s="6"/>
-      <c r="Z78" s="6" t="s">
+      <c r="U78" s="8"/>
+      <c r="V78" s="8"/>
+      <c r="W78" s="8"/>
+      <c r="X78" s="8"/>
+      <c r="Y78" s="8"/>
+      <c r="Z78" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AA78" s="6"/>
-      <c r="AB78" s="6"/>
-      <c r="AC78" s="6"/>
-      <c r="AD78" s="6"/>
-      <c r="AE78" s="6"/>
-      <c r="AF78" s="6"/>
-      <c r="AG78" s="6"/>
-      <c r="AH78" s="6"/>
+      <c r="AA78" s="8"/>
+      <c r="AB78" s="8"/>
+      <c r="AC78" s="8"/>
+      <c r="AD78" s="8"/>
+      <c r="AE78" s="8"/>
+      <c r="AF78" s="8"/>
+      <c r="AG78" s="8"/>
+      <c r="AH78" s="8"/>
     </row>
     <row r="79" spans="6:34" ht="16.8" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="G79" s="7" t="s">
+      <c r="G79" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="H79" s="7"/>
-      <c r="I79" s="7"/>
-      <c r="J79" s="7"/>
-      <c r="K79" s="7"/>
-      <c r="L79" s="7"/>
-      <c r="M79" s="7"/>
-      <c r="N79" s="7" t="s">
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="9"/>
+      <c r="N79" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="O79" s="7"/>
-      <c r="P79" s="7"/>
-      <c r="Q79" s="7"/>
-      <c r="R79" s="7"/>
-      <c r="S79" s="7"/>
-      <c r="T79" s="7" t="s">
+      <c r="O79" s="9"/>
+      <c r="P79" s="9"/>
+      <c r="Q79" s="9"/>
+      <c r="R79" s="9"/>
+      <c r="S79" s="9"/>
+      <c r="T79" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="U79" s="7"/>
-      <c r="V79" s="7"/>
-      <c r="W79" s="7"/>
-      <c r="X79" s="7"/>
-      <c r="Y79" s="7"/>
-      <c r="Z79" s="7" t="s">
+      <c r="U79" s="9"/>
+      <c r="V79" s="9"/>
+      <c r="W79" s="9"/>
+      <c r="X79" s="9"/>
+      <c r="Y79" s="9"/>
+      <c r="Z79" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="AA79" s="7"/>
-      <c r="AB79" s="7"/>
-      <c r="AC79" s="7"/>
-      <c r="AD79" s="7"/>
-      <c r="AE79" s="7"/>
-      <c r="AF79" s="7"/>
-      <c r="AG79" s="7"/>
-      <c r="AH79" s="7"/>
+      <c r="AA79" s="9"/>
+      <c r="AB79" s="9"/>
+      <c r="AC79" s="9"/>
+      <c r="AD79" s="9"/>
+      <c r="AE79" s="9"/>
+      <c r="AF79" s="9"/>
+      <c r="AG79" s="9"/>
+      <c r="AH79" s="9"/>
     </row>
     <row r="80" spans="6:34" x14ac:dyDescent="0.2">
-      <c r="G80" s="5" t="s">
+      <c r="G80" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
-      <c r="J80" s="5"/>
-      <c r="K80" s="5"/>
-      <c r="L80" s="5"/>
-      <c r="M80" s="5"/>
-      <c r="N80" s="5" t="s">
+      <c r="H80" s="7"/>
+      <c r="I80" s="7"/>
+      <c r="J80" s="7"/>
+      <c r="K80" s="7"/>
+      <c r="L80" s="7"/>
+      <c r="M80" s="7"/>
+      <c r="N80" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="O80" s="5"/>
-      <c r="P80" s="5"/>
-      <c r="Q80" s="5"/>
-      <c r="R80" s="5"/>
-      <c r="S80" s="5"/>
-      <c r="T80" s="5" t="s">
+      <c r="O80" s="7"/>
+      <c r="P80" s="7"/>
+      <c r="Q80" s="7"/>
+      <c r="R80" s="7"/>
+      <c r="S80" s="7"/>
+      <c r="T80" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="U80" s="5"/>
-      <c r="V80" s="5"/>
-      <c r="W80" s="5"/>
-      <c r="X80" s="5"/>
-      <c r="Y80" s="5"/>
-      <c r="Z80" s="5" t="s">
+      <c r="U80" s="7"/>
+      <c r="V80" s="7"/>
+      <c r="W80" s="7"/>
+      <c r="X80" s="7"/>
+      <c r="Y80" s="7"/>
+      <c r="Z80" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AA80" s="5"/>
-      <c r="AB80" s="5"/>
-      <c r="AC80" s="5"/>
-      <c r="AD80" s="5"/>
-      <c r="AE80" s="5"/>
-      <c r="AF80" s="5"/>
-      <c r="AG80" s="5"/>
-      <c r="AH80" s="5"/>
+      <c r="AA80" s="7"/>
+      <c r="AB80" s="7"/>
+      <c r="AC80" s="7"/>
+      <c r="AD80" s="7"/>
+      <c r="AE80" s="7"/>
+      <c r="AF80" s="7"/>
+      <c r="AG80" s="7"/>
+      <c r="AH80" s="7"/>
     </row>
     <row r="81" spans="4:34" x14ac:dyDescent="0.2">
-      <c r="G81" s="5" t="s">
+      <c r="G81" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
-      <c r="J81" s="5"/>
-      <c r="K81" s="5"/>
-      <c r="L81" s="5"/>
-      <c r="M81" s="5"/>
-      <c r="N81" s="5" t="s">
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="O81" s="5"/>
-      <c r="P81" s="5"/>
-      <c r="Q81" s="5"/>
-      <c r="R81" s="5"/>
-      <c r="S81" s="5"/>
-      <c r="T81" s="5" t="s">
+      <c r="O81" s="7"/>
+      <c r="P81" s="7"/>
+      <c r="Q81" s="7"/>
+      <c r="R81" s="7"/>
+      <c r="S81" s="7"/>
+      <c r="T81" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="U81" s="5"/>
-      <c r="V81" s="5"/>
-      <c r="W81" s="5"/>
-      <c r="X81" s="5"/>
-      <c r="Y81" s="5"/>
-      <c r="Z81" s="5" t="s">
+      <c r="U81" s="7"/>
+      <c r="V81" s="7"/>
+      <c r="W81" s="7"/>
+      <c r="X81" s="7"/>
+      <c r="Y81" s="7"/>
+      <c r="Z81" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AA81" s="5"/>
-      <c r="AB81" s="5"/>
-      <c r="AC81" s="5"/>
-      <c r="AD81" s="5"/>
-      <c r="AE81" s="5"/>
-      <c r="AF81" s="5"/>
-      <c r="AG81" s="5"/>
-      <c r="AH81" s="5"/>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="7"/>
+      <c r="AC81" s="7"/>
+      <c r="AD81" s="7"/>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="7"/>
+      <c r="AG81" s="7"/>
+      <c r="AH81" s="7"/>
     </row>
     <row r="82" spans="4:34" x14ac:dyDescent="0.2">
-      <c r="G82" s="5" t="s">
+      <c r="G82" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
-      <c r="J82" s="5"/>
-      <c r="K82" s="5"/>
-      <c r="L82" s="5"/>
-      <c r="M82" s="5"/>
-      <c r="N82" s="5" t="s">
+      <c r="H82" s="7"/>
+      <c r="I82" s="7"/>
+      <c r="J82" s="7"/>
+      <c r="K82" s="7"/>
+      <c r="L82" s="7"/>
+      <c r="M82" s="7"/>
+      <c r="N82" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="O82" s="5"/>
-      <c r="P82" s="5"/>
-      <c r="Q82" s="5"/>
-      <c r="R82" s="5"/>
-      <c r="S82" s="5"/>
-      <c r="T82" s="5" t="s">
+      <c r="O82" s="7"/>
+      <c r="P82" s="7"/>
+      <c r="Q82" s="7"/>
+      <c r="R82" s="7"/>
+      <c r="S82" s="7"/>
+      <c r="T82" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="U82" s="5"/>
-      <c r="V82" s="5"/>
-      <c r="W82" s="5"/>
-      <c r="X82" s="5"/>
-      <c r="Y82" s="5"/>
-      <c r="Z82" s="5" t="s">
+      <c r="U82" s="7"/>
+      <c r="V82" s="7"/>
+      <c r="W82" s="7"/>
+      <c r="X82" s="7"/>
+      <c r="Y82" s="7"/>
+      <c r="Z82" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="AA82" s="5"/>
-      <c r="AB82" s="5"/>
-      <c r="AC82" s="5"/>
-      <c r="AD82" s="5"/>
-      <c r="AE82" s="5"/>
-      <c r="AF82" s="5"/>
-      <c r="AG82" s="5"/>
-      <c r="AH82" s="5"/>
+      <c r="AA82" s="7"/>
+      <c r="AB82" s="7"/>
+      <c r="AC82" s="7"/>
+      <c r="AD82" s="7"/>
+      <c r="AE82" s="7"/>
+      <c r="AF82" s="7"/>
+      <c r="AG82" s="7"/>
+      <c r="AH82" s="7"/>
     </row>
     <row r="83" spans="4:34" x14ac:dyDescent="0.2">
-      <c r="G83" s="5" t="s">
+      <c r="G83" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
-      <c r="J83" s="5"/>
-      <c r="K83" s="5"/>
-      <c r="L83" s="5"/>
-      <c r="M83" s="5"/>
-      <c r="N83" s="5" t="s">
+      <c r="H83" s="7"/>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="7"/>
+      <c r="N83" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="O83" s="5"/>
-      <c r="P83" s="5"/>
-      <c r="Q83" s="5"/>
-      <c r="R83" s="5"/>
-      <c r="S83" s="5"/>
-      <c r="T83" s="5" t="s">
+      <c r="O83" s="7"/>
+      <c r="P83" s="7"/>
+      <c r="Q83" s="7"/>
+      <c r="R83" s="7"/>
+      <c r="S83" s="7"/>
+      <c r="T83" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="U83" s="5"/>
-      <c r="V83" s="5"/>
-      <c r="W83" s="5"/>
-      <c r="X83" s="5"/>
-      <c r="Y83" s="5"/>
-      <c r="Z83" s="5" t="s">
+      <c r="U83" s="7"/>
+      <c r="V83" s="7"/>
+      <c r="W83" s="7"/>
+      <c r="X83" s="7"/>
+      <c r="Y83" s="7"/>
+      <c r="Z83" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="AA83" s="5"/>
-      <c r="AB83" s="5"/>
-      <c r="AC83" s="5"/>
-      <c r="AD83" s="5"/>
-      <c r="AE83" s="5"/>
-      <c r="AF83" s="5"/>
-      <c r="AG83" s="5"/>
-      <c r="AH83" s="5"/>
+      <c r="AA83" s="7"/>
+      <c r="AB83" s="7"/>
+      <c r="AC83" s="7"/>
+      <c r="AD83" s="7"/>
+      <c r="AE83" s="7"/>
+      <c r="AF83" s="7"/>
+      <c r="AG83" s="7"/>
+      <c r="AH83" s="7"/>
     </row>
     <row r="85" spans="4:34" x14ac:dyDescent="0.2">
       <c r="D85" s="1" t="s">
@@ -18140,6 +20907,18 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="Z83:AH83"/>
+    <mergeCell ref="T78:Y78"/>
+    <mergeCell ref="T79:Y79"/>
+    <mergeCell ref="T80:Y80"/>
+    <mergeCell ref="T81:Y81"/>
+    <mergeCell ref="T82:Y82"/>
+    <mergeCell ref="T83:Y83"/>
+    <mergeCell ref="Z78:AH78"/>
+    <mergeCell ref="Z79:AH79"/>
+    <mergeCell ref="Z80:AH80"/>
+    <mergeCell ref="Z81:AH81"/>
+    <mergeCell ref="Z82:AH82"/>
     <mergeCell ref="N83:S83"/>
     <mergeCell ref="G78:M78"/>
     <mergeCell ref="G79:M79"/>
@@ -18152,18 +20931,6 @@
     <mergeCell ref="N80:S80"/>
     <mergeCell ref="N81:S81"/>
     <mergeCell ref="N82:S82"/>
-    <mergeCell ref="Z83:AH83"/>
-    <mergeCell ref="T78:Y78"/>
-    <mergeCell ref="T79:Y79"/>
-    <mergeCell ref="T80:Y80"/>
-    <mergeCell ref="T81:Y81"/>
-    <mergeCell ref="T82:Y82"/>
-    <mergeCell ref="T83:Y83"/>
-    <mergeCell ref="Z78:AH78"/>
-    <mergeCell ref="Z79:AH79"/>
-    <mergeCell ref="Z80:AH80"/>
-    <mergeCell ref="Z81:AH81"/>
-    <mergeCell ref="Z82:AH82"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20220125 Build jeus-blog web
・Add StatefulSet, PV and PVC.
</commit_message>
<xml_diff>
--- a/Kubernetes.xlsx
+++ b/Kubernetes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="270">
   <si>
     <t>node&amp;pod確認</t>
     <rPh sb="8" eb="10">
@@ -2735,6 +2735,252 @@
   </si>
   <si>
     <t>HPA（Horizontal Pod Autoscaler)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DaemonSet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DeploymentのreplicasがNode数だけ決まっている形で、Node１つにつき１つだけのPodを生成する</t>
+    <rPh sb="24" eb="25">
+      <t>スウ</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>カタチ</t>
+    </rPh>
+    <rPh sb="54" eb="56">
+      <t>セイセイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>例）Calico Network plugin、kube-proxy、MetalLb speaker</t>
+    <rPh sb="0" eb="1">
+      <t>レイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※Nodeの単一接続するところで、Nodeの外部と通信する。</t>
+    <rPh sb="6" eb="8">
+      <t>タンイツ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>セツゾク</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ガイブ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>ツウシン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-&gt; １つ以上のPodは要らない。１つだけで良い。</t>
+    <rPh sb="6" eb="8">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>イ</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>ヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ConfigMap</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>設定（Conifg)を目的に使用するObject</t>
+    <rPh sb="0" eb="2">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>モクテキ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※環境変数的なもの</t>
+    <rPh sb="1" eb="3">
+      <t>カンキョウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>テキ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PVC, PV</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Claim(要求する)という意味の通り、作成された PV リソースからアサインするためのリソース。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PV はクラスタにボリュームを登録するだけなので Pod から利用する場合には PVC を定義する必要がある。</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PV</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(PersistentVolume, 永続化領域として確保される Volume）</t>
+    </r>
+    <rPh sb="21" eb="23">
+      <t>エイゾク</t>
+    </rPh>
+    <rPh sb="23" eb="24">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>リョウイキ</t>
+    </rPh>
+    <rPh sb="29" eb="31">
+      <t>カクホ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PVC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>（PersistentVolumeClaim）</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>※PVで生成可能なVolume Type</t>
+    <rPh sb="4" eb="6">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>カノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AWS Elastic Block Store, HostPath, NFS, iSCSIなど</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>StatefulSet</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>以前の状態を記憶するセット</t>
+    <rPh sb="0" eb="2">
+      <t>イゼン</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ジョウタイ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>キオク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>各Podが順に生成されるため、固定の名前、Volume、設定などを待つことができる。</t>
+    <rPh sb="0" eb="1">
+      <t>カク</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ジュン</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>セイセイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>コテイ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="33" eb="34">
+      <t>マ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ただし、効率面で良い構造ではないため、要求条件に合わせて適切に利用することが大事。</t>
+    <rPh sb="4" eb="6">
+      <t>コウリツ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>メン</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ヨ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>コウゾウ</t>
+    </rPh>
+    <rPh sb="19" eb="23">
+      <t>ヨウキュウジョウケン</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>ア</t>
+    </rPh>
+    <rPh sb="28" eb="30">
+      <t>テキセツ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ダイジ</t>
+    </rPh>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2901,7 +3147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2912,6 +3158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -14226,13 +14473,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>35859</xdr:colOff>
-      <xdr:row>148</xdr:row>
+      <xdr:row>184</xdr:row>
       <xdr:rowOff>215152</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>1</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:row>186</xdr:row>
       <xdr:rowOff>233083</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -14306,13 +14553,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>35858</xdr:colOff>
-      <xdr:row>152</xdr:row>
+      <xdr:row>188</xdr:row>
       <xdr:rowOff>35858</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>154</xdr:row>
+      <xdr:row>190</xdr:row>
       <xdr:rowOff>53789</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -14417,13 +14664,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>53788</xdr:colOff>
-      <xdr:row>154</xdr:row>
+      <xdr:row>190</xdr:row>
       <xdr:rowOff>80684</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>80683</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>53788</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -14497,13 +14744,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>156</xdr:row>
+      <xdr:row>192</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>62753</xdr:colOff>
-      <xdr:row>158</xdr:row>
+      <xdr:row>194</xdr:row>
       <xdr:rowOff>116541</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -14575,13 +14822,13 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>159</xdr:row>
+      <xdr:row>195</xdr:row>
       <xdr:rowOff>224117</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>62753</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>188258</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -14653,13 +14900,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>67236</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>53787</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>134470</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -14708,13 +14955,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>67236</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>53787</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>160</xdr:row>
+      <xdr:row>196</xdr:row>
       <xdr:rowOff>206187</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -14764,13 +15011,13 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>153</xdr:row>
+      <xdr:row>189</xdr:row>
       <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>62753</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -14816,13 +15063,13 @@
     <xdr:from>
       <xdr:col>25</xdr:col>
       <xdr:colOff>62753</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>75453</xdr:colOff>
-      <xdr:row>160</xdr:row>
+      <xdr:row>196</xdr:row>
       <xdr:rowOff>206188</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -14869,13 +15116,13 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>85165</xdr:colOff>
-      <xdr:row>150</xdr:row>
+      <xdr:row>186</xdr:row>
       <xdr:rowOff>233083</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>85166</xdr:colOff>
-      <xdr:row>152</xdr:row>
+      <xdr:row>188</xdr:row>
       <xdr:rowOff>35858</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -14919,13 +15166,13 @@
     <xdr:from>
       <xdr:col>33</xdr:col>
       <xdr:colOff>17930</xdr:colOff>
-      <xdr:row>148</xdr:row>
+      <xdr:row>184</xdr:row>
       <xdr:rowOff>71717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>119507</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>187</xdr:row>
       <xdr:rowOff>53788</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -14935,7 +15182,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="4455459" y="35894682"/>
+          <a:off x="4455459" y="44608376"/>
           <a:ext cx="773930" cy="708212"/>
           <a:chOff x="2967317" y="17391529"/>
           <a:chExt cx="773930" cy="493059"/>
@@ -15058,13 +15305,13 @@
     <xdr:from>
       <xdr:col>49</xdr:col>
       <xdr:colOff>8964</xdr:colOff>
-      <xdr:row>148</xdr:row>
+      <xdr:row>184</xdr:row>
       <xdr:rowOff>71717</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>55</xdr:col>
       <xdr:colOff>107576</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>187</xdr:row>
       <xdr:rowOff>35858</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -15132,13 +15379,13 @@
     <xdr:from>
       <xdr:col>35</xdr:col>
       <xdr:colOff>107576</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>187</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
       <xdr:colOff>107576</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>179295</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -15184,13 +15431,13 @@
     <xdr:from>
       <xdr:col>52</xdr:col>
       <xdr:colOff>62750</xdr:colOff>
-      <xdr:row>151</xdr:row>
+      <xdr:row>187</xdr:row>
       <xdr:rowOff>71718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
       <xdr:colOff>62750</xdr:colOff>
-      <xdr:row>161</xdr:row>
+      <xdr:row>197</xdr:row>
       <xdr:rowOff>179295</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -15236,13 +15483,13 @@
     <xdr:from>
       <xdr:col>35</xdr:col>
       <xdr:colOff>44823</xdr:colOff>
-      <xdr:row>154</xdr:row>
+      <xdr:row>190</xdr:row>
       <xdr:rowOff>134471</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
       <xdr:colOff>26894</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>215153</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -15298,13 +15545,13 @@
     <xdr:from>
       <xdr:col>35</xdr:col>
       <xdr:colOff>44823</xdr:colOff>
-      <xdr:row>158</xdr:row>
+      <xdr:row>194</xdr:row>
       <xdr:rowOff>116542</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
       <xdr:colOff>26894</xdr:colOff>
-      <xdr:row>159</xdr:row>
+      <xdr:row>195</xdr:row>
       <xdr:rowOff>197224</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -15360,13 +15607,13 @@
     <xdr:from>
       <xdr:col>35</xdr:col>
       <xdr:colOff>116540</xdr:colOff>
-      <xdr:row>153</xdr:row>
+      <xdr:row>189</xdr:row>
       <xdr:rowOff>35859</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>125500</xdr:colOff>
-      <xdr:row>153</xdr:row>
+      <xdr:row>189</xdr:row>
       <xdr:rowOff>35861</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -15407,13 +15654,13 @@
     <xdr:from>
       <xdr:col>51</xdr:col>
       <xdr:colOff>125505</xdr:colOff>
-      <xdr:row>153</xdr:row>
+      <xdr:row>189</xdr:row>
       <xdr:rowOff>35860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
       <xdr:colOff>116541</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>215154</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -15469,13 +15716,13 @@
     <xdr:from>
       <xdr:col>51</xdr:col>
       <xdr:colOff>125505</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>35862</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
       <xdr:colOff>116541</xdr:colOff>
-      <xdr:row>159</xdr:row>
+      <xdr:row>195</xdr:row>
       <xdr:rowOff>215156</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -15531,13 +15778,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>26894</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>53788</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>107576</xdr:colOff>
-      <xdr:row>155</xdr:row>
+      <xdr:row>191</xdr:row>
       <xdr:rowOff>53789</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -15580,13 +15827,13 @@
     <xdr:from>
       <xdr:col>35</xdr:col>
       <xdr:colOff>116540</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>125500</xdr:colOff>
-      <xdr:row>157</xdr:row>
+      <xdr:row>193</xdr:row>
       <xdr:rowOff>44826</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -15627,13 +15874,13 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>26894</xdr:colOff>
-      <xdr:row>159</xdr:row>
+      <xdr:row>195</xdr:row>
       <xdr:rowOff>44824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>107576</xdr:colOff>
-      <xdr:row>159</xdr:row>
+      <xdr:row>195</xdr:row>
       <xdr:rowOff>44825</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -15674,13 +15921,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>134470</xdr:colOff>
-      <xdr:row>175</xdr:row>
+      <xdr:row>211</xdr:row>
       <xdr:rowOff>17931</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
       <xdr:colOff>44824</xdr:colOff>
-      <xdr:row>186</xdr:row>
+      <xdr:row>222</xdr:row>
       <xdr:rowOff>197224</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -15690,7 +15937,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="672352" y="42376166"/>
+          <a:off x="672352" y="51089860"/>
           <a:ext cx="5423648" cy="2841811"/>
           <a:chOff x="1084728" y="41972754"/>
           <a:chExt cx="5423648" cy="2841811"/>
@@ -17046,13 +17293,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>134470</xdr:colOff>
-      <xdr:row>199</xdr:row>
+      <xdr:row>235</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>62</xdr:col>
       <xdr:colOff>98612</xdr:colOff>
-      <xdr:row>216</xdr:row>
+      <xdr:row>252</xdr:row>
       <xdr:rowOff>242046</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -17062,7 +17309,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="672352" y="48167365"/>
+          <a:off x="672352" y="56881059"/>
           <a:ext cx="7763436" cy="4356846"/>
           <a:chOff x="672352" y="48167365"/>
           <a:chExt cx="7763436" cy="4356846"/>
@@ -19432,13 +19679,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>223</xdr:row>
+      <xdr:row>259</xdr:row>
       <xdr:rowOff>89647</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>62</xdr:col>
       <xdr:colOff>98613</xdr:colOff>
-      <xdr:row>240</xdr:row>
+      <xdr:row>276</xdr:row>
       <xdr:rowOff>62751</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -19448,7 +19695,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="672353" y="54066141"/>
+          <a:off x="672353" y="62779835"/>
           <a:ext cx="7763436" cy="4087904"/>
           <a:chOff x="672353" y="54066141"/>
           <a:chExt cx="7763436" cy="4087904"/>
@@ -21257,13 +21504,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>26894</xdr:colOff>
-      <xdr:row>248</xdr:row>
+      <xdr:row>284</xdr:row>
       <xdr:rowOff>233078</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>53</xdr:col>
       <xdr:colOff>76972</xdr:colOff>
-      <xdr:row>268</xdr:row>
+      <xdr:row>304</xdr:row>
       <xdr:rowOff>125506</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -21273,7 +21520,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="833718" y="60260749"/>
+          <a:off x="833718" y="68974443"/>
           <a:ext cx="6370195" cy="4733369"/>
           <a:chOff x="833718" y="60260749"/>
           <a:chExt cx="6370195" cy="4733369"/>
@@ -23203,6 +23450,2170 @@
     </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>125506</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>170328</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>107577</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>233083</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="367" name="직사각형 366"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="932330" y="39866046"/>
+          <a:ext cx="1999129" cy="2725272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>管理者担当</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>107577</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>161366</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>125506</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>179295</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="368" name="그룹 367"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="1048871" y="40099131"/>
+          <a:ext cx="555811" cy="744070"/>
+          <a:chOff x="1210235" y="16324729"/>
+          <a:chExt cx="526452" cy="851647"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="369" name="순서도: 지연 368"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="1284081" y="16750441"/>
+            <a:ext cx="352089" cy="499782"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartDelay">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="370" name="타원 369"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1272315" y="16517918"/>
+            <a:ext cx="388172" cy="371139"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="373" name="TextBox 372"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1244525" y="16324729"/>
+            <a:ext cx="492162" cy="216049"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>管理者</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>188258</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>26894</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>62754</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="58" name="그룹 57"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2017060" y="40610117"/>
+          <a:ext cx="699246" cy="842684"/>
+          <a:chOff x="2456330" y="40959740"/>
+          <a:chExt cx="872098" cy="1107243"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="42" name="순서도: 직접 액세스 저장소 41"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2519082" y="41587271"/>
+            <a:ext cx="797859" cy="179294"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartMagneticDrum">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="43" name="순서도: 자기 디스크 42"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2788024" y="41210754"/>
+            <a:ext cx="170329" cy="475130"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartMagneticDisk">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="39" name="정육면체 38"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2537012" y="40959740"/>
+            <a:ext cx="690282" cy="403412"/>
+          </a:xfrm>
+          <a:prstGeom prst="cube">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>NFS</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="46" name="TextBox 45"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2456330" y="41802423"/>
+            <a:ext cx="872098" cy="264560"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+              <a:t>/nfs_shared</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>125504</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>71714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>116538</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="52" name="그룹 51"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="2142563" y="41945855"/>
+          <a:ext cx="546848" cy="286871"/>
+          <a:chOff x="2483223" y="42537529"/>
+          <a:chExt cx="654424" cy="430306"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="47" name="순서도: 처리 46"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2483223" y="42618212"/>
+            <a:ext cx="537883" cy="349623"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartProcess">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="51" name="순서도: 데이터 50"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2497381" y="42716824"/>
+            <a:ext cx="640266" cy="251011"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartInputOutput">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="379" name="순서도: 처리 378"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2483223" y="42537529"/>
+            <a:ext cx="268941" cy="89648"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartProcess">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>102462</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>204127</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="74" name="꺾인 연결선 73"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="369" idx="1"/>
+          <a:endCxn id="46" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1410415" y="40987529"/>
+          <a:ext cx="508927" cy="704363"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8968</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>206190</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>56367</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>32867</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="386" name="꺾인 연결선 385"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="51" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="1074070" y="41257276"/>
+          <a:ext cx="1278959" cy="988693"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>44824</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>215152</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="619721" cy="275717"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="81" name="TextBox 80"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1389530" y="42089293"/>
+          <a:ext cx="619721" cy="275717"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>PV</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>生成</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>53789</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>53787</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="627529" cy="425758"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="389" name="TextBox 388"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1398495" y="41201787"/>
+          <a:ext cx="627529" cy="425758"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000"/>
+            <a:t>NFS</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000"/>
+            <a:t>生成</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>172</xdr:row>
+      <xdr:rowOff>26893</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="627529" cy="248851"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="390" name="TextBox 389"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2420473" y="41901034"/>
+          <a:ext cx="627529" cy="248851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000"/>
+            <a:t>PV</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>80683</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>62754</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>81295</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>101597</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="85" name="직선 화살표 연결선 84"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="379" idx="3"/>
+          <a:endCxn id="46" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2366683" y="41694848"/>
+          <a:ext cx="612" cy="522937"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>98612</xdr:colOff>
+      <xdr:row>164</xdr:row>
+      <xdr:rowOff>170328</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>233083</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="408" name="직사각형 407"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3460377" y="39866046"/>
+          <a:ext cx="2994211" cy="2725272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>ユーザ（開発者）担当</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>35858</xdr:colOff>
+      <xdr:row>166</xdr:row>
+      <xdr:rowOff>173527</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>80681</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>107576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="411" name="직사각형 410"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3801034" y="40353339"/>
+          <a:ext cx="851647" cy="902237"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+            <a:t>Pods(s)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>80682</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>21127</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>125506</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>197223</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="413" name="직사각형 412"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3711388" y="40442986"/>
+          <a:ext cx="851647" cy="902237"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+            <a:t>Pods(s)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>125506</xdr:colOff>
+      <xdr:row>167</xdr:row>
+      <xdr:rowOff>128704</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>35859</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>62753</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="414" name="직사각형 413"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3621741" y="40550563"/>
+          <a:ext cx="851647" cy="902237"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="tx2">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+            <a:t>Pods(s)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="900"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>125506</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>116543</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>26895</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="204" name="순서도: 자기 디스크 203"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3890682" y="40780449"/>
+          <a:ext cx="546847" cy="394446"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartMagneticDisk">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="bg1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800"/>
+            <a:t>Volume</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>107579</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>35857</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="627529" cy="248851"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="415" name="TextBox 414"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3872755" y="41183857"/>
+          <a:ext cx="627529" cy="248851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>/audit</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1000">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>17928</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>71714</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>26893</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>116538</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="417" name="그룹 416"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="3783104" y="41945855"/>
+          <a:ext cx="546848" cy="286871"/>
+          <a:chOff x="2483223" y="42537529"/>
+          <a:chExt cx="654424" cy="430306"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="418" name="순서도: 처리 417"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2483223" y="42618212"/>
+            <a:ext cx="537883" cy="349623"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartProcess">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="456" name="순서도: 데이터 455"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2497381" y="42716824"/>
+            <a:ext cx="640266" cy="251011"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartInputOutput">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="457" name="순서도: 처리 456"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2483223" y="42537529"/>
+            <a:ext cx="268941" cy="89648"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartProcess">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>125508</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>170327</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="627529" cy="248851"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="458" name="TextBox 457"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3756214" y="41560374"/>
+          <a:ext cx="627529" cy="248851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000"/>
+            <a:t>PVC</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>125506</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>173</xdr:row>
+      <xdr:rowOff>8965</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="461" name="직선 화살표 연결선 460"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4168588" y="41515553"/>
+          <a:ext cx="0" cy="367553"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>53791</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>107574</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="627529" cy="405367"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="462" name="TextBox 461"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2070850" y="42223762"/>
+          <a:ext cx="627529" cy="405367"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000"/>
+            <a:t>nfs-pv</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000"/>
+            <a:t>&lt;100M&gt;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>89649</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>107574</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="627529" cy="405367"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="464" name="TextBox 463"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3720355" y="42223762"/>
+          <a:ext cx="627529" cy="405367"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000"/>
+            <a:t>nfs-pv</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000"/>
+            <a:t>&lt;100M&gt;</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>35855</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>116540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>53784</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>134469</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="465" name="그룹 464"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5683620" y="40054305"/>
+          <a:ext cx="555811" cy="744070"/>
+          <a:chOff x="1210235" y="16324729"/>
+          <a:chExt cx="526452" cy="851647"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="466" name="순서도: 지연 465"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="1284081" y="16750441"/>
+            <a:ext cx="352089" cy="499782"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartDelay">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="469" name="타원 468"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1272315" y="16517918"/>
+            <a:ext cx="388172" cy="371139"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:sysClr val="window" lastClr="FFFFFF"/>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="470" name="TextBox 469"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1244525" y="16324729"/>
+            <a:ext cx="492162" cy="216049"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>開発者</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>107575</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>233082</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>89646</xdr:colOff>
+      <xdr:row>171</xdr:row>
+      <xdr:rowOff>35859</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="472" name="그룹 471"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5486399" y="40896988"/>
+          <a:ext cx="923365" cy="528918"/>
+          <a:chOff x="3436620" y="4907280"/>
+          <a:chExt cx="914400" cy="460205"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="473" name="직사각형 472"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3436620" y="4994105"/>
+            <a:ext cx="906780" cy="373380"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+              <a:t>&gt; kubectl</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+              <a:t>create</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900" baseline="0"/>
+              <a:t> deploy</a:t>
+            </a:r>
+            <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="900"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="478" name="직사각형 477"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="3436620" y="4907280"/>
+            <a:ext cx="914400" cy="103031"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="500"/>
+              <a:t>・・・</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>98612</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>116541</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="479" name="직선 화살표 연결선 478"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4805083" y="40950777"/>
+          <a:ext cx="555811" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>89648</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>26893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>26894</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="480" name="직선 화살표 연결선 479"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2779060" y="42143081"/>
+          <a:ext cx="851646" cy="1"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="38100">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>71720</xdr:colOff>
+      <xdr:row>174</xdr:row>
+      <xdr:rowOff>46291</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="995079" cy="248851"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="481" name="TextBox 480"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2761132" y="42162479"/>
+          <a:ext cx="995079" cy="248851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000"/>
+            <a:t>Bind</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000" baseline="0"/>
+            <a:t> -&gt; Bound</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -23517,11 +25928,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:BM247"/>
+  <dimension ref="D2:BM283"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A238" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BD257" sqref="BD257"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2" defaultRowHeight="19.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -23753,251 +26162,346 @@
         <v>195</v>
       </c>
     </row>
-    <row r="145" spans="4:41" x14ac:dyDescent="0.25">
+    <row r="145" spans="5:8" x14ac:dyDescent="0.25">
       <c r="H145" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="147" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="D147" s="6" t="s">
+    <row r="147" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E147" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="148" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E148" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="149" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F149" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="150" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="G150" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="151" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="H151" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="153" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E153" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="154" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E154" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="155" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F155" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="157" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E157" s="2" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="158" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F158" s="10" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="159" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F159" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="160" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="G160" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="161" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G161" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="163" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F163" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="164" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G164" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="178" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="E178" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="179" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="F179" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="180" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="F180" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="181" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="F181" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="183" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="D183" s="6" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="148" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="E148" t="s">
+    <row r="184" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="E184" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="153" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="T153" t="s">
+    <row r="189" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="T189" t="s">
         <v>199</v>
       </c>
-      <c r="AN153" t="s">
+      <c r="AN189" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="156" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="AO156" t="s">
+    <row r="192" spans="4:41" x14ac:dyDescent="0.25">
+      <c r="AO192" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="158" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="AN158" t="s">
+    <row r="194" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="AN194" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="160" spans="4:41" x14ac:dyDescent="0.25">
-      <c r="AN160" t="s">
+    <row r="196" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="AN196" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="161" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="AP161" t="s">
+    <row r="197" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="AP197" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="163" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="I163" t="s">
+    <row r="199" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="I199" t="s">
         <v>200</v>
       </c>
-      <c r="AJ163" t="s">
+      <c r="AJ199" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="165" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="D165" s="6" t="s">
+    <row r="201" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="D201" s="6" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="166" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="E166" t="s">
+    <row r="202" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="E202" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="168" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="D168" s="6" t="s">
+    <row r="204" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="D204" s="6" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="169" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="E169" t="s">
+    <row r="205" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="E205" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="171" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="E171" s="2" t="s">
+    <row r="207" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="E207" s="2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="172" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="F172" t="s">
+    <row r="208" spans="4:42" x14ac:dyDescent="0.25">
+      <c r="F208" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="173" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="F173" t="s">
+    <row r="209" spans="6:56" x14ac:dyDescent="0.25">
+      <c r="F209" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="174" spans="4:42" x14ac:dyDescent="0.25">
-      <c r="F174" t="s">
+    <row r="210" spans="6:56" x14ac:dyDescent="0.25">
+      <c r="F210" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="180" spans="5:56" x14ac:dyDescent="0.25">
-      <c r="K180" t="s">
+    <row r="216" spans="6:56" x14ac:dyDescent="0.25">
+      <c r="K216" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="185" spans="5:56" x14ac:dyDescent="0.25">
-      <c r="AV185" t="s">
+    <row r="221" spans="6:56" x14ac:dyDescent="0.25">
+      <c r="AV221" t="s">
         <v>216</v>
       </c>
-      <c r="BD185" t="s">
+      <c r="BD221" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="186" spans="5:56" x14ac:dyDescent="0.25">
-      <c r="AV186" t="s">
+    <row r="222" spans="6:56" x14ac:dyDescent="0.25">
+      <c r="AV222" t="s">
         <v>217</v>
       </c>
-      <c r="BD186" t="s">
+      <c r="BD222" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="188" spans="5:56" x14ac:dyDescent="0.25">
-      <c r="R188" t="s">
+    <row r="224" spans="6:56" x14ac:dyDescent="0.25">
+      <c r="R224" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="190" spans="5:56" x14ac:dyDescent="0.25">
-      <c r="E190" s="2" t="s">
+    <row r="226" spans="5:54" x14ac:dyDescent="0.25">
+      <c r="E226" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="191" spans="5:56" x14ac:dyDescent="0.25">
-      <c r="F191" t="s">
+    <row r="227" spans="5:54" x14ac:dyDescent="0.25">
+      <c r="F227" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="192" spans="5:56" x14ac:dyDescent="0.25">
-      <c r="F192" t="s">
+    <row r="228" spans="5:54" x14ac:dyDescent="0.25">
+      <c r="F228" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="193" spans="6:54" x14ac:dyDescent="0.25">
-      <c r="F193" t="s">
+    <row r="229" spans="5:54" x14ac:dyDescent="0.25">
+      <c r="F229" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="194" spans="6:54" x14ac:dyDescent="0.25">
-      <c r="F194" t="s">
+    <row r="230" spans="5:54" x14ac:dyDescent="0.25">
+      <c r="F230" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="196" spans="6:54" x14ac:dyDescent="0.25">
-      <c r="F196" t="s">
+    <row r="232" spans="5:54" x14ac:dyDescent="0.25">
+      <c r="F232" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="197" spans="6:54" x14ac:dyDescent="0.25">
-      <c r="F197" t="s">
+    <row r="233" spans="5:54" x14ac:dyDescent="0.25">
+      <c r="F233" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="198" spans="6:54" x14ac:dyDescent="0.25">
-      <c r="F198" t="s">
+    <row r="234" spans="5:54" x14ac:dyDescent="0.25">
+      <c r="F234" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="201" spans="6:54" x14ac:dyDescent="0.25">
-      <c r="N201" t="s">
+    <row r="237" spans="5:54" x14ac:dyDescent="0.25">
+      <c r="N237" t="s">
         <v>230</v>
       </c>
-      <c r="AA201" s="3" t="s">
+      <c r="AA237" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="AO201" t="s">
+      <c r="AO237" t="s">
         <v>235</v>
       </c>
-      <c r="BB201" s="3" t="s">
+      <c r="BB237" s="3" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="202" spans="6:54" x14ac:dyDescent="0.25">
-      <c r="N202" t="s">
+    <row r="238" spans="5:54" x14ac:dyDescent="0.25">
+      <c r="N238" t="s">
         <v>231</v>
       </c>
-      <c r="AA202" s="3" t="s">
+      <c r="AA238" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="AO202" t="s">
+      <c r="AO238" t="s">
         <v>234</v>
       </c>
-      <c r="BB202" s="3" t="s">
+      <c r="BB238" s="3" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="209" spans="5:65" x14ac:dyDescent="0.25">
-      <c r="BM209" t="s">
+    <row r="245" spans="5:65" x14ac:dyDescent="0.25">
+      <c r="BM245" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="210" spans="5:65" x14ac:dyDescent="0.25">
-      <c r="BM210" t="s">
+    <row r="246" spans="5:65" x14ac:dyDescent="0.25">
+      <c r="BM246" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="220" spans="5:65" x14ac:dyDescent="0.25">
-      <c r="E220" s="2" t="s">
+    <row r="256" spans="5:65" x14ac:dyDescent="0.25">
+      <c r="E256" s="2" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="221" spans="5:65" x14ac:dyDescent="0.25">
-      <c r="F221" t="s">
+    <row r="257" spans="6:40" x14ac:dyDescent="0.25">
+      <c r="F257" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="222" spans="5:65" x14ac:dyDescent="0.25">
-      <c r="F222" t="s">
+    <row r="258" spans="6:40" x14ac:dyDescent="0.25">
+      <c r="F258" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="223" spans="5:65" x14ac:dyDescent="0.25">
-      <c r="G223" t="s">
+    <row r="259" spans="6:40" x14ac:dyDescent="0.25">
+      <c r="G259" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="228" spans="18:40" x14ac:dyDescent="0.25">
-      <c r="R228" t="s">
+    <row r="264" spans="6:40" x14ac:dyDescent="0.25">
+      <c r="R264" t="s">
         <v>244</v>
       </c>
-      <c r="AN228" t="s">
+      <c r="AN264" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="242" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F242" t="s">
+    <row r="278" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F278" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="243" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F243" t="s">
+    <row r="279" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F279" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="244" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="G244" t="s">
+    <row r="280" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="G280" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="246" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E246" s="2" t="s">
+    <row r="282" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="E282" s="2" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="247" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="F247" t="s">
+    <row r="283" spans="5:7" x14ac:dyDescent="0.25">
+      <c r="F283" t="s">
         <v>249</v>
       </c>
     </row>

</xml_diff>